<commit_message>
V2 modify start.py and shell application result to match automation framework
</commit_message>
<xml_diff>
--- a/testset.xlsx
+++ b/testset.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11220" windowWidth="18570" xWindow="5235" yWindow="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11385" windowWidth="21600" xWindow="5400" yWindow="1995"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,13 +16,29 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF00FF00"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <color rgb="0000FF00"/>
+    </font>
+    <font>
+      <color rgb="00FF0000"/>
     </font>
   </fonts>
   <fills count="2">
@@ -45,9 +61,13 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -323,19 +343,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" style="1" width="30.28515625"/>
     <col customWidth="1" max="2" min="2" style="1" width="28.28515625"/>
     <col customWidth="1" max="3" min="3" style="1" width="15.85546875"/>
-    <col customWidth="1" max="13" min="4" style="1" width="9.140625"/>
-    <col customWidth="1" max="16384" min="14" style="1" width="9.140625"/>
+    <col customWidth="1" max="29" min="4" style="1" width="9.140625"/>
+    <col customWidth="1" max="16384" min="30" style="1" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -353,12 +373,24 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>rdp_launch</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
+          <t>app_test</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="inlineStr">
         <is>
           <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>app_test1</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>FAIL</t>
         </is>
       </c>
     </row>

</xml_diff>